<commit_message>
AW - Continued work on the write up
</commit_message>
<xml_diff>
--- a/Advanced Web/Assignment/Design/Test Plan.xlsx
+++ b/Advanced Web/Assignment/Design/Test Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="117">
   <si>
     <t>Location</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>Login should be successful</t>
-  </si>
-  <si>
-    <t>Calendar - Startdard User</t>
   </si>
   <si>
     <t>Events are displayed on the calendar</t>
@@ -379,7 +376,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -414,6 +411,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -803,19 +806,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" customWidth="1"/>
-    <col min="5" max="5" width="48.6640625" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="4" width="56.83203125" customWidth="1"/>
+    <col min="5" max="5" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -855,10 +861,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -875,7 +881,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30">
@@ -895,7 +901,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
@@ -915,7 +921,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
@@ -935,10 +941,10 @@
         <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -955,10 +961,10 @@
         <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -975,7 +981,7 @@
         <v>24</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30">
@@ -995,7 +1001,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30">
@@ -1015,10 +1021,10 @@
         <v>29</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="60">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1035,7 +1041,7 @@
         <v>32</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30">
@@ -1055,7 +1061,7 @@
         <v>35</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30">
@@ -1075,7 +1081,7 @@
         <v>38</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30">
@@ -1095,7 +1101,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30">
@@ -1115,67 +1121,67 @@
         <v>43</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="60">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="F16" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="60">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="F17" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="F18" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30">
@@ -1183,19 +1189,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="F19" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30">
@@ -1203,19 +1209,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="F20" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30">
@@ -1223,59 +1229,59 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="F21" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="F22" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="F23" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30">
@@ -1283,19 +1289,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1303,19 +1309,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="F25" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1323,39 +1329,39 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="F26" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="60">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="F27" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1363,19 +1369,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="F28" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1383,19 +1389,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="F29" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30">
@@ -1403,39 +1409,39 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="F30" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="F31" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="60">
@@ -1443,19 +1449,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="F32" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30">
@@ -1463,59 +1469,59 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="F33" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="F34" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="F35" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="45">
@@ -1523,19 +1529,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="F36" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1543,19 +1549,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="F37" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1563,19 +1569,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="F38" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30">
@@ -1583,19 +1589,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="F39" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="30">
@@ -1603,19 +1609,19 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="F40" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="30">
@@ -1623,87 +1629,88 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="D42" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="F42" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="60">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="45">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="D44" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="F44" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
AW - Updated the report. Also added extra server side validation for updating the users settings
</commit_message>
<xml_diff>
--- a/Advanced Web/Assignment/Design/Test Plan.xlsx
+++ b/Advanced Web/Assignment/Design/Test Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="123">
   <si>
     <t>Location</t>
   </si>
@@ -370,6 +370,24 @@
   </si>
   <si>
     <t>Test 41, and 42 will still pass. With no duplicate dates in the individual boxes. i.e. 5 shifts added for the same day wont display the same entry 5 times, only one will be presented. The same for deleted.</t>
+  </si>
+  <si>
+    <t>Ensure that the Copy &amp; Paste functionality works correctly</t>
+  </si>
+  <si>
+    <t>Login as the admin user. Click on a day that has staff shifts on, and click Copy. Clcick on a day that you want to shifts copied onto. Click Paste</t>
+  </si>
+  <si>
+    <t>The day which Paste was clicked on, will match the shifts that were on the original day that was copied.</t>
+  </si>
+  <si>
+    <t>Ensure that the calendar view is displayed correctly</t>
+  </si>
+  <si>
+    <t>When logged in as the standard user, the calendar view should match that described in the assignment brief.</t>
+  </si>
+  <si>
+    <t>4 full weeks should be displayed, commencing with the following Monday (it should not be possible to see the current week)</t>
   </si>
 </sst>
 </file>
@@ -809,10 +827,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1704,6 +1722,46 @@
         <v>76</v>
       </c>
     </row>
+    <row r="45" spans="1:6" ht="45">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>